<commit_message>
Added indexing/steps. Tweaks to indexing.
</commit_message>
<xml_diff>
--- a/test/instron-test-files/data/processed/data (stage=raw | item=tracking | v0).xlsx
+++ b/test/instron-test-files/data/processed/data (stage=raw | item=tracking | v0).xlsx
@@ -108,22 +108,22 @@
     <t>N</t>
   </si>
   <si>
-    <t>step_1.0_step</t>
-  </si>
-  <si>
-    <t>step_1.0_stop</t>
-  </si>
-  <si>
-    <t>step_1.0_start</t>
+    <t>step_1_start</t>
+  </si>
+  <si>
+    <t>step_1_stop</t>
+  </si>
+  <si>
+    <t>step_1_step</t>
+  </si>
+  <si>
+    <t>step_-1_start</t>
+  </si>
+  <si>
+    <t>step_-1_stop</t>
   </si>
   <si>
     <t>step_-1_step</t>
-  </si>
-  <si>
-    <t>step_-1_stop</t>
-  </si>
-  <si>
-    <t>step_-1_start</t>
   </si>
 </sst>
 </file>
@@ -897,7 +897,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -919,7 +919,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -930,7 +930,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -952,7 +952,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved indexing. Add prefix idx_ for ints.
</commit_message>
<xml_diff>
--- a/test/instron-test-files/data/processed/data (stage=raw | item=tracking | v0).xlsx
+++ b/test/instron-test-files/data/processed/data (stage=raw | item=tracking | v0).xlsx
@@ -108,10 +108,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>step_1</t>
-  </si>
-  <si>
-    <t>step_-1</t>
+    <t>step.idx_1</t>
+  </si>
+  <si>
+    <t>step.idx_neg_1</t>
   </si>
 </sst>
 </file>

</xml_diff>